<commit_message>
- Support to read inlineStr type cell value, relate issue #208, PR #209; - go test and godoc has been updated
</commit_message>
<xml_diff>
--- a/test/Book1.xlsx
+++ b/test/Book1.xlsx
@@ -2593,6 +2593,11 @@
         <v>2</v>
       </c>
       <c r="D1" s="2"/>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>inlineStr</t>
+        </is>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
- Initialize shared formula types support, relate issue #227; - go test and godoc has been updated
</commit_message>
<xml_diff>
--- a/test/Book1.xlsx
+++ b/test/Book1.xlsx
@@ -2702,6 +2702,21 @@
       <c r="D11" s="4">
         <v>37</v>
       </c>
+      <c r="E11" s="4">
+        <f t="normal">B2+B3</f>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" ref="F11:H11" si="0">IF(B2&gt;0, (D2/B2)*100, 0)</f>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" ref="G11:I11" si="1">IF(B2&gt;0, (D2/B2)*100, 0)</f>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="1"/>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
resolve #276, add OfficeOpenXML-XMLSchema-Strict mode support
</commit_message>
<xml_diff>
--- a/test/Book1.xlsx
+++ b/test/Book1.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuri/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13220" yWindow="6260" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="16880" windowWidth="28160" xWindow="13220" yWindow="6260"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" relationships:id="rId1"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" relationships:id="rId2"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="3" relationships:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="false"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -155,11 +151,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="177" formatCode="General"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,12 +189,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -206,8 +208,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill/>
+    <fill/>
+    <fill/>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -217,45 +222,75 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
+        <color theme="2" tint="-0.09994811853389081"/>
       </left>
       <right style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
+        <color theme="2" tint="-0.09994811853389081"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
+        <color theme="2" tint="-0.09994811853389081"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
+        <color theme="2" tint="-0.09994811853389081"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="8">
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="177" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="2" fillId="3" fontId="0" numFmtId="22" xfId="0">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="21" xfId="0">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="4" fillId="5" fontId="0" numFmtId="22" xfId="0">
+      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2521,27 +2556,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A19:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" width="5" max="6" min="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="0" width="5"/>
   </cols>
   <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10">
+      <c r="G10">
+        <f>SUM(Sheet1!B19,Sheet1!C19)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <f>SUM(Sheet2!D2,Sheet2!D11)</f>
-        <v>237</v>
-      </c>
-    </row>
+      </c>
+      <c r="C19">
+        <f>SUM(Sheet2!D2,Sheet2!D9)</f>
+      </c>
+    </row>
+    <row r="20"/>
     <row r="21" spans="1:4">
       <c r="C21" t="s">
         <v>18</v>
@@ -2550,43 +2611,311 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" customHeight="1" ht="25">
+    <row customHeight="true" ht="25" r="22" spans="1:4">
       <c r="A22" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27">
+      <c r="B27" t="str">
+        <v>cell</v>
+      </c>
+      <c r="C27" t="str"/>
+      <c r="D27">
+        <v>42</v>
+      </c>
+      <c r="E27">
+        <v>42</v>
+      </c>
+      <c r="F27" s="7">
+        <v>43390.019016186365</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="D11:F13"/>
+    <mergeCell ref="G10:K12"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A22" r:id="rId1"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A22" relationships:id="rId1"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId7"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId8"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <picture r:id="rId4"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId2"/>
+  <legacyDrawing xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId3"/>
+  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230">
+      <c r="B230" t="str">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col customWidth="1" width="0.5" max="3" min="3"/>
-    <col max="7" min="7" style="0"/>
-    <col customWidth="1" width="0" max="9" min="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="0.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="9" min="9" style="0" width="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
+    <row ht="17" r="1" spans="1:4">
+      <c r="A1" s="1">
+        <v>100</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
@@ -2598,8 +2927,14 @@
           <t>inlineStr</t>
         </is>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="F1" t="str" xml:space="preserve">
+        <v> Hello</v>
+      </c>
+      <c r="G1" t="str">
+        <v>World</v>
+      </c>
+    </row>
+    <row ht="17" r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2612,8 +2947,13 @@
       <c r="D2" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>42</v>
+      </c>
+      <c r="G2" t="str"/>
+      <c r="M2" t="str"/>
+    </row>
+    <row ht="17" r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2626,8 +2966,11 @@
       <c r="D3" s="4">
         <v>450</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>127</v>
+      </c>
+    </row>
+    <row ht="17" r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2640,8 +2983,14 @@
       <c r="D4" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>32767</v>
+      </c>
+      <c r="G4" s="5">
+        <v>43390.01900236038</v>
+      </c>
+    </row>
+    <row ht="17" r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -2654,59 +3003,81 @@
       <c r="D5" s="4">
         <v>510</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>2147483647</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.11574074</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4">
         <v>315</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>2147483647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="4">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>42.65418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="4">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2" customHeight="1" ht="0">
+      <c r="F8">
+        <v>-42.65418</v>
+      </c>
+    </row>
+    <row customHeight="true" r="9" spans="1:4">
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="4">
         <v>348</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="C11" s="4" t="str">
-        <v>Other</v>
-      </c>
-      <c r="D11" s="4">
-        <v>37</v>
+        <v>Knowns</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <v>ccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccc</v>
       </c>
       <c r="E11" s="4">
         <f t="normal">B2+B3</f>
       </c>
       <c r="F11" s="4">
         <f t="shared" ref="F11:H11" si="0">IF(B2&gt;0, (D2/B2)*100, 0)</f>
+        <v>4294967295</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" ref="G11:I11" si="1">IF(B2&gt;0, (D2/B2)*100, 0)</f>
@@ -2718,11 +3089,1570 @@
         <f t="shared" si="1"/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:4">
+      <c r="F12">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="F13">
+        <v>65535</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="F14">
+        <v>4294967295</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="F15">
+        <v>4294967295</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="F17" t="str">
+        <v>(5+10i)</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId1"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="C1" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="str">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="str">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="str">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="str">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="str">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="str">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="str">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="str">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="str">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="str">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="str">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="str">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="str">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="str">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="str">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="str">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="C23" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="str">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="str">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="str">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" t="str">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="str">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="str">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="str">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" t="str">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="str">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" t="str">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" t="str">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" t="str">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="C36" t="str">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" t="str">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="C38" t="str">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="C39" t="str">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" t="str">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" t="str">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" t="str">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" t="str">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" t="str">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="C45" t="str">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" t="str">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="C47" t="str">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="C48" t="str">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="C49" t="str">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" t="str">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="C51" t="str">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="C52" t="str">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" t="str">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="C54" t="str">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="C55" t="str">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="C56" t="str">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="C57" t="str">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="C58" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="C59" t="str">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" t="str">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="C61" t="str">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="C62" t="str">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="C63" t="str">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="C64" t="str">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="C65" t="str">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="C66" t="str">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="C67" t="str">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="C68" t="str">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="C69" t="str">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="C70" t="str">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="C71" t="str">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="C72" t="str">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="C73" t="str">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="C74" t="str">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="C75" t="str">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="C76" t="str">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="C77" t="str">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="C78" t="str">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="C79" t="str">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="C80" t="str">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="C81" t="str">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="C82" t="str">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="C83" t="str">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="C84" t="str">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="C85" t="str">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="C86" t="str">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="C87" t="str">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="C88" t="str">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="C89" t="str">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="C90" t="str">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="C91" t="str">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="C92" t="str">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="C93" t="str">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="C94" t="str">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="C95" t="str">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="C96" t="str">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="C97" t="str">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="C98" t="str">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="C99" t="str">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="C100" t="str">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="C101" t="str">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="C102" t="str">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="C103" t="str">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="C104" t="str">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="C105" t="str">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="C106" t="str">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="C107" t="str">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="C108" t="str">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="C109" t="str">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="C110" t="str">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="C111" t="str">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="C112" t="str">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="C113" t="str">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="C114" t="str">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="C115" t="str">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="C116" t="str">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="C117" t="str">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="C118" t="str">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="C119" t="str">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="C120" t="str">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="C121" t="str">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="C122" t="str">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="C123" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="C124" t="str">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="C125" t="str">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="C126" t="str">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="C127" t="str">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="C128" t="str">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="C129" t="str">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="C130" t="str">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="C131" t="str">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="C132" t="str">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="C133" t="str">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="C134" t="str">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="C135" t="str">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="C136" t="str">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="C137" t="str">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="C138" t="str">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="C139" t="str">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="C140" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="C141" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="C142" t="str">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="C143" t="str">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="C144" t="str">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="C145" t="str">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="C146" t="str">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="C147" t="str">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="C148" t="str">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="C149" t="str">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="C150" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="C151" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="C152" t="str">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="C153" t="str">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="C154" t="str">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="C155" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="C156" t="str">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="C157" t="str">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="C158" t="str">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="C159" t="str">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="C160" t="str">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="C161" t="str">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="C162" t="str">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="C163" t="str">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="C164" t="str">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="C165" t="str">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="C166" t="str">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="C167" t="str">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="C168" t="str">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="C169" t="str">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="C170" t="str">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="C171" t="str">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="C172" t="str">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="C173" t="str">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="C174" t="str">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="C175" t="str">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="C176" t="str">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="C177" t="str">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="C178" t="str">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="C179" t="str">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="C180" t="str">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="C181" t="str">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="C182" t="str">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="C183" t="str">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="C184" t="str">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="C185" t="str">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="C186" t="str">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="C187" t="str">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="C188" t="str">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="C189" t="str">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="C190" t="str">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="C191" t="str">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="C192" t="str">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="C193" t="str">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="C194" t="str">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="C195" t="str">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="C196" t="str">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="C197" t="str">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="C198" t="str">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="C199" t="str">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="C200" t="str">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="C201" t="str">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="C202" t="str">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="C203" t="str">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="C204" t="str">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="C205" t="str">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="C206" t="str">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="C207" t="str">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="C208" t="str">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="C209" t="str">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="C210" t="str">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="C211" t="str">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="C212" t="str">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="C213" t="str">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="C214" t="str">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="C215" t="str">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="C216" t="str">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="C217" t="str">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="C218" t="str">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="C219" t="str">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="C220" t="str">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="C221" t="str">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="C222" t="str">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="C223" t="str">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="C224" t="str">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="C225" t="str">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="C226" t="str">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="C227" t="str">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="C228" t="str">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="C229" t="str">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="B230" t="str">
+        <v>10</v>
+      </c>
+      <c r="C230" t="str">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="C231" t="str">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="C232" t="str">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="C233" t="str">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="C234" t="str">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="C235" t="str">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="C236" t="str">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="C237" t="str">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="C238" t="str">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="C239" t="str">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="C240" t="str">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="C241" t="str">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="C242" t="str">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="C243" t="str">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="C244" t="str">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="C245" t="str">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="C246" t="str">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="C247" t="str">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="C248" t="str">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="C249" t="str">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="C250" t="str">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="C251" t="str">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="C252" t="str">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="C253" t="str">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="C254" t="str">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="C255" t="str">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="C256" t="str">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="C257" t="str">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="C258" t="str">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="C259" t="str">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="C260" t="str">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="C261" t="str">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="C262" t="str">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="C263" t="str">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="C264" t="str">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="C265" t="str">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="C266" t="str">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="C267" t="str">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="C268" t="str">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="C269" t="str">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="C270" t="str">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="C271" t="str">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="C272" t="str">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="C273" t="str">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="C274" t="str">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="C275" t="str">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="C276" t="str">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="C277" t="str">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="C278" t="str">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="C279" t="str">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="C280" t="str">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="C281" t="str">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="C282" t="str">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="C283" t="str">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="C284" t="str">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="C285" t="str">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="C286" t="str">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="C287" t="str">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="C288" t="str">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="C289" t="str">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="C290" t="str">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="C291" t="str">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="C292" t="str">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="C293" t="str">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="C294" t="str">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="C295" t="str">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="C296" t="str">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="C297" t="str">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="C298" t="str">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="C299" t="str">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="C300" t="str">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
resolve #273 new feature: protect sheet support
new feature: protect sheet support, relate issue #273
</commit_message>
<xml_diff>
--- a/test/Book1.xlsx
+++ b/test/Book1.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuri/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="16880" windowWidth="28160" xWindow="13220" yWindow="6260"/>
+    <workbookView xWindow="13220" yWindow="6260" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" relationships:id="rId1"/>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" relationships:id="rId2"/>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="3" relationships:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="false"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -151,11 +155,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="177" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,18 +193,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
-      <patternFill patternType="none">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -208,11 +206,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill/>
-    <fill/>
-    <fill/>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -222,75 +217,45 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.09994811853389081"/>
+        <color theme="2" tint="-9.9948118533890809E-2"/>
       </left>
       <right style="thin">
-        <color theme="2" tint="-0.09994811853389081"/>
+        <color theme="2" tint="-9.9948118533890809E-2"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-0.09994811853389081"/>
+        <color theme="2" tint="-9.9948118533890809E-2"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.09994811853389081"/>
+        <color theme="2" tint="-9.9948118533890809E-2"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="177" xfId="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="2" fillId="3" fontId="0" numFmtId="22" xfId="0">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="21" xfId="0">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="4" fillId="5" fontId="0" numFmtId="22" xfId="0">
-      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2556,53 +2521,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A19:D22"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="0" width="5"/>
+    <col customWidth="1" width="5" max="6" min="6"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10">
-      <c r="G10">
-        <f>SUM(Sheet1!B19,Sheet1!C19)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <f>SUM(Sheet2!D2,Sheet2!D11)</f>
-      </c>
-      <c r="C19">
-        <f>SUM(Sheet2!D2,Sheet2!D9)</f>
+        <v>237</v>
       </c>
     </row>
-    <row r="20"/>
     <row r="21" spans="1:4">
       <c r="C21" t="s">
         <v>18</v>
@@ -2611,311 +2550,43 @@
         <v>19</v>
       </c>
     </row>
-    <row customHeight="true" ht="25" r="22" spans="1:4">
+    <row r="22" spans="1:4" customHeight="1" ht="25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27">
-      <c r="B27" t="str">
-        <v>cell</v>
-      </c>
-      <c r="C27" t="str"/>
-      <c r="D27">
-        <v>42</v>
-      </c>
-      <c r="E27">
-        <v>42</v>
-      </c>
-      <c r="F27" s="7">
-        <v>43390.019016186365</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells>
-    <mergeCell ref="D11:F13"/>
-    <mergeCell ref="G10:K12"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A22" relationships:id="rId1"/>
-    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId7"/>
-    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId8"/>
+    <hyperlink ref="A22" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <drawing xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId2"/>
-  <legacyDrawing xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId3"/>
-  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <picture r:id="rId4"/>
   <tableParts count="1">
-    <tablePart xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId5"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref=""/>
-  <sheetViews/>
-  <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
-    <row r="200"/>
-    <row r="201"/>
-    <row r="202"/>
-    <row r="203"/>
-    <row r="204"/>
-    <row r="205"/>
-    <row r="206"/>
-    <row r="207"/>
-    <row r="208"/>
-    <row r="209"/>
-    <row r="210"/>
-    <row r="211"/>
-    <row r="212"/>
-    <row r="213"/>
-    <row r="214"/>
-    <row r="215"/>
-    <row r="216"/>
-    <row r="217"/>
-    <row r="218"/>
-    <row r="219"/>
-    <row r="220"/>
-    <row r="221"/>
-    <row r="222"/>
-    <row r="223"/>
-    <row r="224"/>
-    <row r="225"/>
-    <row r="226"/>
-    <row r="227"/>
-    <row r="228"/>
-    <row r="229"/>
-    <row r="230">
-      <c r="B230" t="str">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="0.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="0"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="9" min="9" style="0" width="0"/>
+    <col customWidth="1" width="0.5" max="3" min="3"/>
+    <col max="7" min="7" style="0"/>
+    <col customWidth="1" width="0" max="9" min="9"/>
   </cols>
   <sheetData>
-    <row ht="17" r="1" spans="1:4">
-      <c r="A1" s="1">
-        <v>100</v>
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
@@ -2927,14 +2598,8 @@
           <t>inlineStr</t>
         </is>
       </c>
-      <c r="F1" t="str" xml:space="preserve">
-        <v> Hello</v>
-      </c>
-      <c r="G1" t="str">
-        <v>World</v>
-      </c>
     </row>
-    <row ht="17" r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2947,13 +2612,8 @@
       <c r="D2" s="4">
         <v>200</v>
       </c>
-      <c r="F2">
-        <v>42</v>
-      </c>
-      <c r="G2" t="str"/>
-      <c r="M2" t="str"/>
     </row>
-    <row ht="17" r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2966,11 +2626,8 @@
       <c r="D3" s="4">
         <v>450</v>
       </c>
-      <c r="F3">
-        <v>127</v>
-      </c>
     </row>
-    <row ht="17" r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2983,14 +2640,8 @@
       <c r="D4" s="4">
         <v>200</v>
       </c>
-      <c r="F4">
-        <v>32767</v>
-      </c>
-      <c r="G4" s="5">
-        <v>43390.01900236038</v>
-      </c>
     </row>
-    <row ht="17" r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -3003,81 +2654,59 @@
       <c r="D5" s="4">
         <v>510</v>
       </c>
-      <c r="F5">
-        <v>2147483647</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0.11574074</v>
-      </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4">
         <v>315</v>
       </c>
-      <c r="F6">
-        <v>2147483647</v>
-      </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="4">
         <v>127</v>
       </c>
-      <c r="F7">
-        <v>42.65418</v>
-      </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="4">
         <v>89</v>
       </c>
-      <c r="F8">
-        <v>-42.65418</v>
-      </c>
     </row>
-    <row customHeight="true" r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2" customHeight="1" ht="0">
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="4">
         <v>348</v>
       </c>
-      <c r="F9">
-        <v>42</v>
-      </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="4">
         <v>53</v>
       </c>
-      <c r="F10">
-        <v>42</v>
-      </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="str">
-        <v>Knowns</v>
-      </c>
-      <c r="D11" s="4" t="str">
-        <v>ccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccc</v>
+        <v>Other</v>
+      </c>
+      <c r="D11" s="4">
+        <v>37</v>
       </c>
       <c r="E11" s="4">
         <f t="normal">B2+B3</f>
       </c>
       <c r="F11" s="4">
         <f t="shared" ref="F11:H11" si="0">IF(B2&gt;0, (D2/B2)*100, 0)</f>
-        <v>4294967295</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" ref="G11:I11" si="1">IF(B2&gt;0, (D2/B2)*100, 0)</f>
@@ -3089,1570 +2718,11 @@
         <f t="shared" si="1"/>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="F12">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="F13">
-        <v>65535</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="F14">
-        <v>4294967295</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="F15">
-        <v>4294967295</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="F17" t="str">
-        <v>(5+10i)</v>
-      </c>
-    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A6"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId1"/>
-    <hyperlink ref="D6" location="Sheet1!D8"/>
-  </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="C1" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="C2" t="str">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" t="str">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="C4" t="str">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="str">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="str">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="str">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" t="str">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" t="str">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" t="str">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" t="str">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" t="str">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" t="str">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" t="str">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" t="str">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" t="str">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="C17" t="str">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" t="str">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" t="str">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="C21" t="str">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" t="str">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="C23" t="str">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="C24" t="str">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="C25" t="str">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="C26" t="str">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" t="str">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" t="str">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" t="str">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" t="str">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="C31" t="str">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="C32" t="str">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" t="str">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="C34" t="str">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="C35" t="str">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="C36" t="str">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" t="str">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="C38" t="str">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="C39" t="str">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="C40" t="str">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="C41" t="str">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="C42" t="str">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="C43" t="str">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="C44" t="str">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="C45" t="str">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="C46" t="str">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="C47" t="str">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="C48" t="str">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="C49" t="str">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="C50" t="str">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="C51" t="str">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="C52" t="str">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="C53" t="str">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="C54" t="str">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="C55" t="str">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="C56" t="str">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="C57" t="str">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="C58" t="str">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="C59" t="str">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="C60" t="str">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="C61" t="str">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="C62" t="str">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="C63" t="str">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="C64" t="str">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="C65" t="str">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="C66" t="str">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="C67" t="str">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="C68" t="str">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="C69" t="str">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="C70" t="str">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="C71" t="str">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="C72" t="str">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="C73" t="str">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="C74" t="str">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="C75" t="str">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="C76" t="str">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="C77" t="str">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="C78" t="str">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="C79" t="str">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="C80" t="str">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="C81" t="str">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="C82" t="str">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="C83" t="str">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="C84" t="str">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="C85" t="str">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="C86" t="str">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="C87" t="str">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="C88" t="str">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="C89" t="str">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="C90" t="str">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="C91" t="str">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="C92" t="str">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="C93" t="str">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="C94" t="str">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="C95" t="str">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="C96" t="str">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="C97" t="str">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="C98" t="str">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="C99" t="str">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="C100" t="str">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="C101" t="str">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="C102" t="str">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="C103" t="str">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="C104" t="str">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="C105" t="str">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="C106" t="str">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="C107" t="str">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="C108" t="str">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="C109" t="str">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="C110" t="str">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="C111" t="str">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="C112" t="str">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="C113" t="str">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="C114" t="str">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="C115" t="str">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="C116" t="str">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="C117" t="str">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="C118" t="str">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="C119" t="str">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="C120" t="str">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="C121" t="str">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="C122" t="str">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="C123" t="str">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="C124" t="str">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="C125" t="str">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="C126" t="str">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="C127" t="str">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="C128" t="str">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="C129" t="str">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="C130" t="str">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="C131" t="str">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="C132" t="str">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="C133" t="str">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="C134" t="str">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="C135" t="str">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="C136" t="str">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="C137" t="str">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="C138" t="str">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="C139" t="str">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="C140" t="str">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="C141" t="str">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="C142" t="str">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="C143" t="str">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="C144" t="str">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="C145" t="str">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="C146" t="str">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="C147" t="str">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="C148" t="str">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="C149" t="str">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="C150" t="str">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="C151" t="str">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="C152" t="str">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="C153" t="str">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="C154" t="str">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="C155" t="str">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="C156" t="str">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="C157" t="str">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="C158" t="str">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="C159" t="str">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="C160" t="str">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="C161" t="str">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="C162" t="str">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="C163" t="str">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="C164" t="str">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="C165" t="str">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="C166" t="str">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="C167" t="str">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="C168" t="str">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="C169" t="str">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="C170" t="str">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="C171" t="str">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="C172" t="str">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="C173" t="str">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="C174" t="str">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="C175" t="str">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="C176" t="str">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="C177" t="str">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="C178" t="str">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="C179" t="str">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="C180" t="str">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="C181" t="str">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="C182" t="str">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="C183" t="str">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="C184" t="str">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="C185" t="str">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="C186" t="str">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="C187" t="str">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="C188" t="str">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="C189" t="str">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="C190" t="str">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="C191" t="str">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="C192" t="str">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="C193" t="str">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="C194" t="str">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="C195" t="str">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="C196" t="str">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="C197" t="str">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="C198" t="str">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="C199" t="str">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="C200" t="str">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="C201" t="str">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="C202" t="str">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="C203" t="str">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="C204" t="str">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="C205" t="str">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="C206" t="str">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="C207" t="str">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="C208" t="str">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="C209" t="str">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="C210" t="str">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="C211" t="str">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="C212" t="str">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="C213" t="str">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="C214" t="str">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="C215" t="str">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="C216" t="str">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="C217" t="str">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="C218" t="str">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="C219" t="str">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="C220" t="str">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="C221" t="str">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="C222" t="str">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="C223" t="str">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="C224" t="str">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="C225" t="str">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="C226" t="str">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="C227" t="str">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="C228" t="str">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="C229" t="str">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="B230" t="str">
-        <v>10</v>
-      </c>
-      <c r="C230" t="str">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="C231" t="str">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="C232" t="str">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="C233" t="str">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="C234" t="str">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="C235" t="str">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="C236" t="str">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="C237" t="str">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="C238" t="str">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="C239" t="str">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="C240" t="str">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="C241" t="str">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="C242" t="str">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="C243" t="str">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="C244" t="str">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="C245" t="str">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="C246" t="str">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="C247" t="str">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="C248" t="str">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="C249" t="str">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="C250" t="str">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="C251" t="str">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="C252" t="str">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="C253" t="str">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="C254" t="str">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="C255" t="str">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="C256" t="str">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="C257" t="str">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="C258" t="str">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="C259" t="str">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="C260" t="str">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="C261" t="str">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="C262" t="str">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="C263" t="str">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="C264" t="str">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="C265" t="str">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="C266" t="str">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="C267" t="str">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="C268" t="str">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="C269" t="str">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="C270" t="str">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="C271" t="str">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="C272" t="str">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="C273" t="str">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="C274" t="str">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="C275" t="str">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="C276" t="str">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="C277" t="str">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="C278" t="str">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="C279" t="str">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="C280" t="str">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="C281" t="str">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="C282" t="str">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="C283" t="str">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="C284" t="str">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="C285" t="str">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="C286" t="str">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="C287" t="str">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="C288" t="str">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="C289" t="str">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="290">
-      <c r="C290" t="str">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="291">
-      <c r="C291" t="str">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="292">
-      <c r="C292" t="str">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="293">
-      <c r="C293" t="str">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="294">
-      <c r="C294" t="str">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="295">
-      <c r="C295" t="str">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="296">
-      <c r="C296" t="str">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="297">
-      <c r="C297" t="str">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="298">
-      <c r="C298" t="str">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="299">
-      <c r="C299" t="str">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="300">
-      <c r="C300" t="str">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref=""/>
-  <sheetViews/>
-  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>